<commit_message>
upd testing kern. objects with kern save in json file
</commit_message>
<xml_diff>
--- a/reports/xlsx/granichnoe.xlsx
+++ b/reports/xlsx/granichnoe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5208"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Месторождение</t>
   </si>
@@ -39,6 +39,9 @@
     <t>количество залежей</t>
   </si>
   <si>
+    <t>керн</t>
+  </si>
+  <si>
     <t>Граничное месторождение</t>
   </si>
   <si>
@@ -51,16 +54,10 @@
     <t>нурлатский район республика татарстан</t>
   </si>
   <si>
-    <t>башкирский верейский каширский</t>
-  </si>
-  <si>
-    <t>глава 2.1, id = 118</t>
-  </si>
-  <si>
-    <t>из указанной главы (введение)</t>
-  </si>
-  <si>
-    <t>(не вывел нужные объекты)</t>
+    <t>башкирский-верейский-каширский</t>
+  </si>
+  <si>
+    <t>нет</t>
   </si>
 </sst>
 </file>
@@ -81,24 +78,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -128,21 +113,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -447,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,13 +435,13 @@
     <col min="2" max="2" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -484,54 +460,37 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F4:G4"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>